<commit_message>
[data] service keywords + review dataset
</commit_message>
<xml_diff>
--- a/dataset/bean_review.xlsx
+++ b/dataset/bean_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\beanBot\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73EE988-D318-412F-B8CE-818EED4B06D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7882EEB-CB49-4CC5-AA11-84421C5F53F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="5303" windowWidth="13980" windowHeight="9532" xr2:uid="{85867CEE-1CD5-4227-9657-02A573F6A235}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{85867CEE-1CD5-4227-9657-02A573F6A235}"/>
   </bookViews>
   <sheets>
     <sheet name="cooking" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="processed" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="143">
   <si>
     <t>sID</t>
   </si>
@@ -403,6 +404,72 @@
   </si>
   <si>
     <t>eu</t>
+  </si>
+  <si>
+    <t>mcgill student's nightline</t>
+  </si>
+  <si>
+    <t>the buddy program</t>
+  </si>
+  <si>
+    <t>project 10 listening line</t>
+  </si>
+  <si>
+    <t>therapist assisted online</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>not helfpful at all!</t>
+  </si>
+  <si>
+    <t>perfectly solve my problem</t>
+  </si>
+  <si>
+    <t>phd support group</t>
+  </si>
+  <si>
+    <t>a waste of time</t>
+  </si>
+  <si>
+    <t>intersting outcome, maybe this is the benefit of having someone to talk to</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>sacomss support groups</t>
+  </si>
+  <si>
+    <t>timeCommit</t>
+  </si>
+  <si>
+    <t>urgency</t>
+  </si>
+  <si>
+    <t>professional</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>in-person</t>
+  </si>
+  <si>
+    <t>drop-in and talk to someone</t>
   </si>
 </sst>
 </file>
@@ -475,12 +542,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{156B1564-3B09-4420-BC02-DE7F40A4A916}" name="Table13" displayName="Table13" ref="A1:L43" totalsRowShown="0">
-  <autoFilter ref="A1:L43" xr:uid="{7DAB65E2-6F33-4DB9-A913-FD6F85245948}"/>
-  <sortState ref="A2:L37">
-    <sortCondition descending="1" ref="A1:A37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{156B1564-3B09-4420-BC02-DE7F40A4A916}" name="Table13" displayName="Table13" ref="A1:P75" totalsRowShown="0">
+  <autoFilter ref="A1:P75" xr:uid="{7DAB65E2-6F33-4DB9-A913-FD6F85245948}"/>
+  <sortState ref="A2:P75">
+    <sortCondition ref="A1:A75"/>
   </sortState>
-  <tableColumns count="12">
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{5C4085D0-8BF5-4784-831B-CC7DE8641506}" name="sID"/>
     <tableColumn id="2" xr3:uid="{BB11D204-3916-448A-8E92-0CD9B81EB701}" name="sName"/>
     <tableColumn id="3" xr3:uid="{74003699-1241-4078-AE3D-C61A9FE36BEF}" name="faculty"/>
@@ -489,6 +556,10 @@
     <tableColumn id="6" xr3:uid="{D93F6109-DCB1-4AC4-A715-9F515AA6FFD9}" name="international"/>
     <tableColumn id="7" xr3:uid="{E430D158-271A-42FE-A1F7-CA0922217496}" name="language"/>
     <tableColumn id="8" xr3:uid="{2E78D8F4-3E74-4F62-9F73-6BD54C1AC326}" name="cultural_bg"/>
+    <tableColumn id="14" xr3:uid="{046A0331-A420-4553-9F17-E03C489A8256}" name="timeCommit"/>
+    <tableColumn id="16" xr3:uid="{59C46896-6CBB-4B75-9411-F0FD93B79940}" name="urgency"/>
+    <tableColumn id="15" xr3:uid="{E3424582-9168-41FB-BC34-07C1AA9469DA}" name="professional"/>
+    <tableColumn id="13" xr3:uid="{BFAE9EC4-5249-4EE2-AE95-EB1016A1EE16}" name="medium"/>
     <tableColumn id="9" xr3:uid="{82DC2025-D802-4F77-83B3-8824CCC24ED1}" name="s_score"/>
     <tableColumn id="10" xr3:uid="{E01F1A4D-4211-48C3-A875-6D4EF749977D}" name="m_score"/>
     <tableColumn id="11" xr3:uid="{92B66EE2-3781-4061-8A70-362C8C7D5A8E}" name="goal"/>
@@ -819,25 +890,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F1D709-E284-4020-9295-69C8984861A6}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="49.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.06640625" customWidth="1"/>
     <col min="6" max="6" width="12.796875" customWidth="1"/>
     <col min="7" max="7" width="9.73046875" customWidth="1"/>
-    <col min="8" max="8" width="11.46484375" customWidth="1"/>
-    <col min="10" max="10" width="9.19921875" customWidth="1"/>
+    <col min="8" max="12" width="11.46484375" customWidth="1"/>
+    <col min="14" max="14" width="9.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -863,24 +934,36 @@
         <v>13</v>
       </c>
       <c r="I1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -895,71 +978,95 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M3">
+        <v>2.5</v>
+      </c>
+      <c r="N3">
+        <v>2.5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -968,74 +1075,98 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>141</v>
+      </c>
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
         <v>105</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
+        <v>89</v>
+      </c>
+      <c r="I5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -1044,109 +1175,139 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>141</v>
+      </c>
+      <c r="M6">
         <v>2</v>
       </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-      <c r="K6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9">
         <v>2</v>
       </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>10</v>
-      </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1158,346 +1319,454 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
         <v>105</v>
       </c>
       <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>141</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>79</v>
+      </c>
+      <c r="P10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" t="s">
         <v>19</v>
       </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10">
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>141</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="J10">
-        <v>4</v>
-      </c>
-      <c r="K10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>3</v>
-      </c>
-      <c r="K12" t="s">
-        <v>53</v>
-      </c>
-      <c r="L12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
+      <c r="O15" t="s">
+        <v>82</v>
+      </c>
+      <c r="P15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
         <v>2</v>
       </c>
-      <c r="K14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15">
-        <v>5</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16">
-        <v>5</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
-      </c>
-      <c r="K16" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="O16" t="s">
+        <v>84</v>
+      </c>
+      <c r="P16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="L17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>5</v>
+      </c>
+      <c r="O17" t="s">
+        <v>85</v>
+      </c>
+      <c r="P17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
@@ -1506,68 +1775,80 @@
         <v>105</v>
       </c>
       <c r="H18" t="s">
-        <v>120</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
+        <v>139</v>
+      </c>
+      <c r="J18" t="s">
+        <v>18</v>
       </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" t="s">
         <v>105</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19">
-        <v>5</v>
-      </c>
-      <c r="J19">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="I19" t="s">
+        <v>139</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
       </c>
       <c r="K19" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -1576,36 +1857,42 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>105</v>
       </c>
       <c r="H20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20">
+        <v>120</v>
+      </c>
+      <c r="I20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20">
         <v>2</v>
       </c>
-      <c r="J20">
-        <v>3</v>
-      </c>
-      <c r="K20" t="s">
-        <v>68</v>
-      </c>
-      <c r="L20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
@@ -1620,60 +1907,72 @@
         <v>105</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-      <c r="J21">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>139</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
       </c>
       <c r="K21" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="L21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>139</v>
+      </c>
+      <c r="J22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" t="s">
+        <v>141</v>
+      </c>
+      <c r="M22">
         <v>3</v>
       </c>
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22">
-        <v>5</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="K22" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1698,124 +1997,169 @@
       <c r="H23" t="s">
         <v>19</v>
       </c>
-      <c r="I23">
-        <v>4</v>
-      </c>
-      <c r="J23">
-        <v>4</v>
+      <c r="I23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" t="s">
+        <v>18</v>
       </c>
       <c r="K23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="O23" t="s">
         <v>78</v>
       </c>
-      <c r="L23" t="s">
+      <c r="P23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>141</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24">
-        <v>5</v>
-      </c>
-      <c r="J24">
-        <v>5</v>
-      </c>
-      <c r="K24" t="s">
-        <v>35</v>
-      </c>
-      <c r="L24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
       <c r="D25" t="s">
         <v>16</v>
       </c>
       <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" t="s">
+        <v>141</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
         <v>14</v>
       </c>
-      <c r="F25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25">
-        <v>2.5</v>
-      </c>
-      <c r="J25">
-        <v>2.5</v>
-      </c>
-      <c r="K25" t="s">
-        <v>25</v>
-      </c>
-      <c r="L25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="I26" t="s">
+        <v>139</v>
+      </c>
+      <c r="J26" t="s">
+        <v>10</v>
       </c>
       <c r="K26" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="L26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>1</v>
+      </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1835,57 +2179,93 @@
       <c r="H27" t="s">
         <v>37</v>
       </c>
+      <c r="I27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" t="s">
+        <v>18</v>
+      </c>
       <c r="K27" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" t="s">
+        <v>138</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+      <c r="O27" t="s">
         <v>38</v>
       </c>
-      <c r="L27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="P27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>6</v>
+      </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H28" t="s">
-        <v>89</v>
+        <v>18</v>
+      </c>
+      <c r="I28" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" t="s">
+        <v>18</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="L28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="N28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>6</v>
+      </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29" t="s">
         <v>18</v>
@@ -1893,45 +2273,75 @@
       <c r="H29" t="s">
         <v>18</v>
       </c>
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" t="s">
+        <v>18</v>
+      </c>
       <c r="K29" t="s">
         <v>18</v>
       </c>
       <c r="L29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>6</v>
+      </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="I30" t="s">
+        <v>139</v>
+      </c>
+      <c r="J30" t="s">
+        <v>9</v>
       </c>
       <c r="K30" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="L30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>6</v>
+      </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
         <v>31</v>
@@ -1951,16 +2361,37 @@
       <c r="H31" t="s">
         <v>18</v>
       </c>
+      <c r="I31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" t="s">
+        <v>18</v>
+      </c>
       <c r="K31" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" t="s">
+        <v>138</v>
+      </c>
+      <c r="M31">
+        <v>5</v>
+      </c>
+      <c r="N31">
+        <v>5</v>
+      </c>
+      <c r="O31" t="s">
         <v>77</v>
       </c>
-      <c r="L31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="P31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>6</v>
+      </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
@@ -1969,59 +2400,89 @@
         <v>16</v>
       </c>
       <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" t="s">
         <v>14</v>
       </c>
-      <c r="F32" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" t="s">
-        <v>91</v>
-      </c>
-      <c r="K32" t="s">
-        <v>79</v>
-      </c>
-      <c r="L32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" t="s">
-        <v>15</v>
-      </c>
       <c r="F33" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="H33" t="s">
-        <v>92</v>
+        <v>18</v>
+      </c>
+      <c r="I33" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" t="s">
+        <v>18</v>
       </c>
       <c r="K33" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="L33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M33">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>6</v>
+      </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
@@ -2033,10 +2494,16 @@
         <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="H34" t="s">
-        <v>57</v>
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" t="s">
+        <v>18</v>
       </c>
       <c r="K34" t="s">
         <v>18</v>
@@ -2044,13 +2511,22 @@
       <c r="L34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M34">
+        <v>5</v>
+      </c>
+      <c r="N34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>7</v>
+      </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
         <v>16</v>
@@ -2059,7 +2535,7 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G35" t="s">
         <v>18</v>
@@ -2067,28 +2543,40 @@
       <c r="H35" t="s">
         <v>18</v>
       </c>
+      <c r="I35" t="s">
+        <v>140</v>
+      </c>
+      <c r="J35" t="s">
+        <v>9</v>
+      </c>
       <c r="K35" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="L35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
         <v>9</v>
@@ -2099,19 +2587,34 @@
       <c r="H36" t="s">
         <v>18</v>
       </c>
+      <c r="I36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" t="s">
+        <v>18</v>
+      </c>
       <c r="K36" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="L36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M36">
+        <v>4</v>
+      </c>
+      <c r="N36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>7</v>
+      </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
         <v>16</v>
@@ -2126,16 +2629,34 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" t="s">
+        <v>9</v>
       </c>
       <c r="K37" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="L37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+      <c r="M37">
+        <v>5</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
@@ -2154,8 +2675,38 @@
       <c r="H38" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38" t="s">
+        <v>138</v>
+      </c>
+      <c r="M38">
+        <v>3</v>
+      </c>
+      <c r="N38">
+        <v>5</v>
+      </c>
+      <c r="O38" t="s">
+        <v>18</v>
+      </c>
+      <c r="P38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -2174,8 +2725,38 @@
       <c r="H39" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" t="s">
+        <v>138</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="O39" t="s">
+        <v>18</v>
+      </c>
+      <c r="P39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>123</v>
+      </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
@@ -2194,8 +2775,38 @@
       <c r="H40" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I40" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" t="s">
+        <v>18</v>
+      </c>
+      <c r="K40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" t="s">
+        <v>138</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>5</v>
+      </c>
+      <c r="O40" t="s">
+        <v>18</v>
+      </c>
+      <c r="P40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
       <c r="C41" t="s">
         <v>39</v>
       </c>
@@ -2214,8 +2825,38 @@
       <c r="H41" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I41" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" t="s">
+        <v>10</v>
+      </c>
+      <c r="L41" t="s">
+        <v>138</v>
+      </c>
+      <c r="M41">
+        <v>5</v>
+      </c>
+      <c r="N41">
+        <v>3</v>
+      </c>
+      <c r="O41" t="s">
+        <v>18</v>
+      </c>
+      <c r="P41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
       <c r="C42" t="s">
         <v>60</v>
       </c>
@@ -2234,8 +2875,38 @@
       <c r="H42" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42" t="s">
+        <v>138</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42" t="s">
+        <v>18</v>
+      </c>
+      <c r="P42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>122</v>
+      </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
@@ -2254,10 +2925,1562 @@
       <c r="H43" t="s">
         <v>57</v>
       </c>
+      <c r="I43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
+        <v>10</v>
+      </c>
+      <c r="L43" t="s">
+        <v>18</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="O43" t="s">
+        <v>18</v>
+      </c>
+      <c r="P43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" t="s">
+        <v>126</v>
+      </c>
+      <c r="H44" t="s">
+        <v>120</v>
+      </c>
+      <c r="I44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" t="s">
+        <v>138</v>
+      </c>
+      <c r="M44">
+        <v>5</v>
+      </c>
+      <c r="N44">
+        <v>5</v>
+      </c>
+      <c r="O44" t="s">
+        <v>18</v>
+      </c>
+      <c r="P44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>105</v>
+      </c>
+      <c r="H45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" t="s">
+        <v>18</v>
+      </c>
+      <c r="L45" t="s">
+        <v>138</v>
+      </c>
+      <c r="M45">
+        <v>5</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" t="s">
+        <v>105</v>
+      </c>
+      <c r="H46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" t="s">
+        <v>140</v>
+      </c>
+      <c r="J46" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" t="s">
+        <v>141</v>
+      </c>
+      <c r="M46">
+        <v>4</v>
+      </c>
+      <c r="N46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47" t="s">
+        <v>140</v>
+      </c>
+      <c r="J47" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" t="s">
+        <v>141</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" t="s">
+        <v>140</v>
+      </c>
+      <c r="J48" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" t="s">
+        <v>141</v>
+      </c>
+      <c r="M48">
+        <v>2</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" t="s">
+        <v>140</v>
+      </c>
+      <c r="J49" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" t="s">
+        <v>141</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" t="s">
+        <v>140</v>
+      </c>
+      <c r="J50" t="s">
+        <v>18</v>
+      </c>
+      <c r="K50" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" t="s">
+        <v>141</v>
+      </c>
+      <c r="M50">
+        <v>5</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" t="s">
+        <v>126</v>
+      </c>
+      <c r="H51" t="s">
+        <v>57</v>
+      </c>
+      <c r="I51" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51" t="s">
+        <v>18</v>
+      </c>
+      <c r="L51" t="s">
+        <v>138</v>
+      </c>
+      <c r="M51">
+        <v>5</v>
+      </c>
+      <c r="N51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" t="s">
+        <v>139</v>
+      </c>
+      <c r="J52" t="s">
+        <v>9</v>
+      </c>
+      <c r="K52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" t="s">
+        <v>138</v>
+      </c>
+      <c r="M52">
+        <v>3</v>
+      </c>
+      <c r="N52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" t="s">
+        <v>139</v>
+      </c>
+      <c r="J53" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53" t="s">
+        <v>18</v>
+      </c>
+      <c r="L53" t="s">
+        <v>138</v>
+      </c>
+      <c r="M53">
+        <v>5</v>
+      </c>
+      <c r="N53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" t="s">
+        <v>139</v>
+      </c>
+      <c r="J54" t="s">
+        <v>18</v>
+      </c>
+      <c r="K54" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54" t="s">
+        <v>138</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="N54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" t="s">
+        <v>139</v>
+      </c>
+      <c r="J55" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" t="s">
+        <v>138</v>
+      </c>
+      <c r="M55">
+        <v>4</v>
+      </c>
+      <c r="N55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" t="s">
+        <v>139</v>
+      </c>
+      <c r="J56" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56" t="s">
+        <v>18</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" t="s">
+        <v>105</v>
+      </c>
+      <c r="H57" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57" t="s">
+        <v>140</v>
+      </c>
+      <c r="J57" t="s">
+        <v>10</v>
+      </c>
+      <c r="K57" t="s">
+        <v>9</v>
+      </c>
+      <c r="L57" t="s">
+        <v>141</v>
+      </c>
+      <c r="M57">
+        <v>5</v>
+      </c>
+      <c r="N57">
+        <v>5</v>
+      </c>
+      <c r="O57" t="s">
+        <v>65</v>
+      </c>
+      <c r="P57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" t="s">
+        <v>105</v>
+      </c>
+      <c r="H58" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" t="s">
+        <v>140</v>
+      </c>
+      <c r="J58" t="s">
+        <v>10</v>
+      </c>
+      <c r="K58" t="s">
+        <v>9</v>
+      </c>
+      <c r="L58" t="s">
+        <v>141</v>
+      </c>
+      <c r="M58">
+        <v>5</v>
+      </c>
+      <c r="N58">
+        <v>5</v>
+      </c>
+      <c r="O58" t="s">
+        <v>27</v>
+      </c>
+      <c r="P58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" t="s">
+        <v>140</v>
+      </c>
+      <c r="J59" t="s">
+        <v>18</v>
+      </c>
+      <c r="K59" t="s">
+        <v>9</v>
+      </c>
+      <c r="L59" t="s">
+        <v>18</v>
+      </c>
+      <c r="M59">
+        <v>2</v>
+      </c>
+      <c r="N59">
+        <v>3</v>
+      </c>
+      <c r="O59" t="s">
+        <v>68</v>
+      </c>
+      <c r="P59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" t="s">
+        <v>105</v>
+      </c>
+      <c r="H60" t="s">
+        <v>19</v>
+      </c>
+      <c r="I60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" t="s">
+        <v>10</v>
+      </c>
+      <c r="K60" t="s">
+        <v>9</v>
+      </c>
+      <c r="L60" t="s">
+        <v>18</v>
+      </c>
+      <c r="M60">
+        <v>3</v>
+      </c>
+      <c r="N60">
+        <v>3</v>
+      </c>
+      <c r="O60" t="s">
+        <v>35</v>
+      </c>
+      <c r="P60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" t="s">
+        <v>105</v>
+      </c>
+      <c r="H61" t="s">
+        <v>48</v>
+      </c>
+      <c r="I61" t="s">
+        <v>140</v>
+      </c>
+      <c r="J61" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" t="s">
+        <v>9</v>
+      </c>
+      <c r="L61" t="s">
+        <v>18</v>
+      </c>
+      <c r="M61">
+        <v>2</v>
+      </c>
+      <c r="N61">
+        <v>3</v>
+      </c>
+      <c r="O61" t="s">
+        <v>47</v>
+      </c>
+      <c r="P61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" t="s">
+        <v>105</v>
+      </c>
+      <c r="H62" t="s">
+        <v>19</v>
+      </c>
+      <c r="I62" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" t="s">
+        <v>9</v>
+      </c>
+      <c r="L62" t="s">
+        <v>141</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <v>5</v>
+      </c>
+      <c r="O62" t="s">
+        <v>21</v>
+      </c>
+      <c r="P62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" t="s">
+        <v>105</v>
+      </c>
+      <c r="H63" t="s">
+        <v>19</v>
+      </c>
+      <c r="I63" t="s">
+        <v>140</v>
+      </c>
+      <c r="J63" t="s">
+        <v>9</v>
+      </c>
+      <c r="K63" t="s">
+        <v>9</v>
+      </c>
+      <c r="L63" t="s">
+        <v>141</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>4</v>
+      </c>
+      <c r="O63" t="s">
+        <v>23</v>
+      </c>
+      <c r="P63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" t="s">
+        <v>105</v>
+      </c>
+      <c r="H64" t="s">
+        <v>19</v>
+      </c>
+      <c r="I64" t="s">
+        <v>140</v>
+      </c>
+      <c r="J64" t="s">
+        <v>10</v>
+      </c>
+      <c r="K64" t="s">
+        <v>9</v>
+      </c>
+      <c r="L64" t="s">
+        <v>141</v>
+      </c>
+      <c r="M64">
+        <v>5</v>
+      </c>
+      <c r="N64">
+        <v>5</v>
+      </c>
+      <c r="O64" t="s">
+        <v>27</v>
+      </c>
+      <c r="P64" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" t="s">
+        <v>105</v>
+      </c>
+      <c r="H65" t="s">
+        <v>19</v>
+      </c>
+      <c r="I65" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" t="s">
+        <v>10</v>
+      </c>
+      <c r="K65" t="s">
+        <v>9</v>
+      </c>
+      <c r="L65" t="s">
+        <v>141</v>
+      </c>
+      <c r="M65">
+        <v>3</v>
+      </c>
+      <c r="N65">
+        <v>4</v>
+      </c>
+      <c r="O65" t="s">
+        <v>29</v>
+      </c>
+      <c r="P65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" t="s">
+        <v>18</v>
+      </c>
+      <c r="H66" t="s">
+        <v>90</v>
+      </c>
+      <c r="I66" t="s">
+        <v>140</v>
+      </c>
+      <c r="J66" t="s">
+        <v>10</v>
+      </c>
+      <c r="K66" t="s">
+        <v>9</v>
+      </c>
+      <c r="L66" t="s">
+        <v>141</v>
+      </c>
+      <c r="M66">
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <v>4</v>
+      </c>
+      <c r="O66" t="s">
+        <v>42</v>
+      </c>
+      <c r="P66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H67" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K67" t="s">
+        <v>9</v>
+      </c>
+      <c r="L67" t="s">
+        <v>18</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>3</v>
+      </c>
+      <c r="O67" t="s">
+        <v>53</v>
+      </c>
+      <c r="P67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" t="s">
+        <v>120</v>
+      </c>
+      <c r="I68" t="s">
+        <v>139</v>
+      </c>
+      <c r="J68" t="s">
+        <v>9</v>
+      </c>
+      <c r="K68" t="s">
+        <v>9</v>
+      </c>
+      <c r="L68" t="s">
+        <v>141</v>
+      </c>
+      <c r="M68">
+        <v>1</v>
+      </c>
+      <c r="N68">
+        <v>1</v>
+      </c>
+      <c r="O68" t="s">
+        <v>64</v>
+      </c>
+      <c r="P68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>99</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>18</v>
+      </c>
+      <c r="H69" t="s">
+        <v>93</v>
+      </c>
+      <c r="I69" t="s">
+        <v>139</v>
+      </c>
+      <c r="J69" t="s">
+        <v>9</v>
+      </c>
+      <c r="K69" t="s">
+        <v>9</v>
+      </c>
+      <c r="L69" t="s">
+        <v>18</v>
+      </c>
+      <c r="M69">
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <v>2</v>
+      </c>
+      <c r="O69" t="s">
+        <v>69</v>
+      </c>
+      <c r="P69" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>99</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K70" t="s">
+        <v>9</v>
+      </c>
+      <c r="L70" t="s">
+        <v>18</v>
+      </c>
+      <c r="M70">
+        <v>5</v>
+      </c>
+      <c r="N70">
+        <v>5</v>
+      </c>
+      <c r="O70" t="s">
+        <v>83</v>
+      </c>
+      <c r="P70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>99</v>
+      </c>
+      <c r="C71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" t="s">
+        <v>105</v>
+      </c>
+      <c r="H71" t="s">
+        <v>43</v>
+      </c>
+      <c r="I71" t="s">
+        <v>140</v>
+      </c>
+      <c r="J71" t="s">
+        <v>10</v>
+      </c>
+      <c r="K71" t="s">
+        <v>9</v>
+      </c>
+      <c r="L71" t="s">
+        <v>18</v>
+      </c>
+      <c r="M71">
+        <v>5</v>
+      </c>
+      <c r="N71">
+        <v>5</v>
+      </c>
+      <c r="O71" t="s">
+        <v>18</v>
+      </c>
+      <c r="P71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" t="s">
+        <v>106</v>
+      </c>
+      <c r="H72" t="s">
+        <v>57</v>
+      </c>
+      <c r="I72" t="s">
+        <v>140</v>
+      </c>
+      <c r="J72" t="s">
+        <v>10</v>
+      </c>
+      <c r="K72" t="s">
+        <v>9</v>
+      </c>
+      <c r="L72" t="s">
+        <v>18</v>
+      </c>
+      <c r="M72">
+        <v>5</v>
+      </c>
+      <c r="N72">
+        <v>5</v>
+      </c>
+      <c r="O72" t="s">
+        <v>81</v>
+      </c>
+      <c r="P72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" t="s">
+        <v>50</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" t="s">
+        <v>105</v>
+      </c>
+      <c r="H73" t="s">
+        <v>120</v>
+      </c>
+      <c r="I73" t="s">
+        <v>140</v>
+      </c>
+      <c r="J73" t="s">
+        <v>10</v>
+      </c>
+      <c r="K73" t="s">
+        <v>9</v>
+      </c>
+      <c r="L73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M73">
+        <v>5</v>
+      </c>
+      <c r="N73">
+        <v>4</v>
+      </c>
+      <c r="O73" t="s">
+        <v>54</v>
+      </c>
+      <c r="P73" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>10</v>
+      </c>
+      <c r="B74" t="s">
+        <v>99</v>
+      </c>
+      <c r="C74" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" t="s">
+        <v>105</v>
+      </c>
+      <c r="H74" t="s">
+        <v>19</v>
+      </c>
+      <c r="I74" t="s">
+        <v>140</v>
+      </c>
+      <c r="J74" t="s">
+        <v>10</v>
+      </c>
+      <c r="K74" t="s">
+        <v>9</v>
+      </c>
+      <c r="L74" t="s">
+        <v>18</v>
+      </c>
+      <c r="M74">
+        <v>5</v>
+      </c>
+      <c r="N74">
+        <v>5</v>
+      </c>
+      <c r="O74" t="s">
+        <v>66</v>
+      </c>
+      <c r="P74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75" t="s">
+        <v>99</v>
+      </c>
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>105</v>
+      </c>
+      <c r="H75" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" t="s">
+        <v>139</v>
+      </c>
+      <c r="J75" t="s">
+        <v>10</v>
+      </c>
+      <c r="K75" t="s">
+        <v>9</v>
+      </c>
+      <c r="L75" t="s">
+        <v>141</v>
+      </c>
+      <c r="M75">
+        <v>2</v>
+      </c>
+      <c r="N75">
+        <v>3</v>
+      </c>
+      <c r="O75" t="s">
+        <v>68</v>
+      </c>
+      <c r="P75" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="nan">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="nan">
       <formula>LEFT(A1,LEN("nan"))="nan"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2385,7 +4608,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D2" sqref="C2:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3698,7 +5921,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="nan">
+    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="nan">
       <formula>LEFT(A1,LEN("nan"))="nan"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>